<commit_message>
final test case file added
</commit_message>
<xml_diff>
--- a/Testing_assignments/QuizAppUsecases_Devanathan.xlsx
+++ b/Testing_assignments/QuizAppUsecases_Devanathan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devanathan.k\Documents\changepondtraining\Assignments\Testing_assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t>Revision History</t>
   </si>
@@ -205,21 +205,12 @@
     <t>v1.0</t>
   </si>
   <si>
-    <t>sanjay</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hematite Portal </t>
   </si>
   <si>
-    <t>Kishore</t>
-  </si>
-  <si>
     <t>v1.1</t>
   </si>
   <si>
-    <t>Tarun</t>
-  </si>
-  <si>
     <t>v1.2</t>
   </si>
   <si>
@@ -229,10 +220,10 @@
     <t>v1.3</t>
   </si>
   <si>
-    <t>santoz</t>
-  </si>
-  <si>
     <t>Use case diagram</t>
+  </si>
+  <si>
+    <t>Monica</t>
   </si>
 </sst>
 </file>
@@ -240,7 +231,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -707,39 +698,61 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -755,11 +768,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -767,42 +783,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1141,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,13 +1147,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
       <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1189,80 +1180,80 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="66">
+      <c r="C3" s="34">
         <v>45615</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>64</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="36">
+        <v>45615</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="68">
-        <v>45615</v>
-      </c>
-      <c r="D4" s="71" t="s">
+      <c r="E4" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>64</v>
-      </c>
-      <c r="E4" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="70" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="68">
+      <c r="B5" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="36">
         <v>45615</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="68">
+      <c r="B6" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="36">
         <v>45615</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>64</v>
-      </c>
-      <c r="E6" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="70" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1322,52 +1313,52 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="60"/>
+      <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="49"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="55"/>
+      <c r="B7" s="51"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="55"/>
+      <c r="B8" s="51"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="45"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="45"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="53"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="48"/>
+      <c r="B12" s="56"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -1376,74 +1367,74 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="57"/>
       <c r="B23" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="56" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="65" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="66"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
@@ -1474,46 +1465,46 @@
       <c r="F29" s="16"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="51"/>
+      <c r="B30" s="59"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="63"/>
+      <c r="B31" s="67"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="63"/>
+      <c r="B32" s="67"/>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="64"/>
+      <c r="B33" s="68"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="65"/>
+      <c r="B34" s="43"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="65"/>
+      <c r="B35" s="43"/>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="53"/>
+      <c r="B36" s="61"/>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
@@ -1540,10 +1531,10 @@
       <c r="B40" s="24"/>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="42"/>
+      <c r="B41" s="62"/>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
@@ -1592,40 +1583,40 @@
       <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="42"/>
+      <c r="B50" s="62"/>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
-      <c r="B51" s="38"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="64"/>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
-      <c r="B52" s="55"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="51"/>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
-      <c r="B53" s="55"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="51"/>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
-      <c r="B54" s="55"/>
+      <c r="A54" s="50"/>
+      <c r="B54" s="51"/>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39"/>
-      <c r="B55" s="40"/>
+      <c r="A55" s="54"/>
+      <c r="B55" s="55"/>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="40"/>
+      <c r="A56" s="54"/>
+      <c r="B56" s="55"/>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="42"/>
+      <c r="B57" s="62"/>
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
@@ -1640,68 +1631,68 @@
       <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
+      <c r="A60" s="69"/>
       <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
+      <c r="A61" s="70"/>
       <c r="B61" s="8"/>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
+      <c r="A62" s="70"/>
       <c r="B62" s="8"/>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
+      <c r="A63" s="70"/>
       <c r="B63" s="8"/>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
+      <c r="A64" s="70"/>
       <c r="B64" s="8"/>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
+      <c r="A65" s="70"/>
       <c r="B65" s="8"/>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="44"/>
+      <c r="A66" s="70"/>
       <c r="B66" s="6"/>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="44"/>
+      <c r="A67" s="70"/>
       <c r="B67" s="8"/>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="44"/>
+      <c r="A68" s="70"/>
       <c r="B68" s="8"/>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
+      <c r="A69" s="70"/>
       <c r="B69" s="8"/>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
+      <c r="A70" s="70"/>
       <c r="B70" s="8"/>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="45"/>
+      <c r="A71" s="71"/>
       <c r="B71" s="8"/>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="42"/>
+      <c r="B72" s="62"/>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="41" t="s">
+      <c r="A74" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="42"/>
+      <c r="B74" s="62"/>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
@@ -1712,16 +1703,16 @@
       <c r="B76" s="6"/>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B77" s="42"/>
+      <c r="B77" s="62"/>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B78" s="38"/>
+      <c r="B78" s="64"/>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1741,15 +1732,13 @@
     <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A60:A71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A77:B77"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:A25"/>
@@ -1765,13 +1754,15 @@
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A60:A71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1782,7 +1773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1793,7 +1784,7 @@
   <sheetData>
     <row r="1" spans="9:15" x14ac:dyDescent="0.25">
       <c r="I1" s="72" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J1" s="73"/>
       <c r="K1" s="73"/>

</xml_diff>